<commit_message>
Atualização dos componentes com a correção.
</commit_message>
<xml_diff>
--- a/Jupyter/whatCemig/Envios.xlsx
+++ b/Jupyter/whatCemig/Envios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atanaufo\Documents\GitHub\python\Jupyter\whatCemig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DF4E6E-7C11-4E5C-841B-E3DA506C5027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42A0ED8-8D25-4861-A45C-C9043E9C7218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{35571D8A-49AD-4B5E-837F-295801CCF79C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>nome</t>
   </si>
@@ -60,13 +60,25 @@
   </si>
   <si>
     <t>5531998542933</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Olá é um tratativa de erro. Fulano</t>
+  </si>
+  <si>
+    <t>filho</t>
+  </si>
+  <si>
+    <t>Boa noite meu Fulano. Espero que esteja tudo bem contigo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +88,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -103,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -112,6 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,11 +467,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B093489-00C6-41DF-B636-C1457D746588}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,7 +509,39 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>5531996514243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização final - 30/03/2024.
</commit_message>
<xml_diff>
--- a/Jupyter/whatCemig/Envios.xlsx
+++ b/Jupyter/whatCemig/Envios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atanaufo\Documents\GitHub\python\Jupyter\whatCemig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42A0ED8-8D25-4861-A45C-C9043E9C7218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A38FD52-18BA-4A32-A9B3-C9490A49F3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{35571D8A-49AD-4B5E-837F-295801CCF79C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>nome</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Boa noite meu Fulano. Espero que esteja tudo bem contigo.</t>
+  </si>
+  <si>
+    <t>transferir.png</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,7 +506,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>

</xml_diff>